<commit_message>
Focus area added to the Leaders page
</commit_message>
<xml_diff>
--- a/data/UoB_Agreements.xlsx
+++ b/data/UoB_Agreements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97333\Desktop\Hawra\Cloud Computing\ITCC481\Partnership\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275F697A-425A-4E23-8EA4-D0CB52998815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041E8D1B-F1BA-4904-82F1-3DFA1BA15A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agreements Master Sheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="202">
   <si>
     <t>Record ID</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>https://www.undp.org</t>
-  </si>
-  <si>
-    <t>https://www.undp.org/sites/g/files/zskgke326/files/media_asset/undp-logo-blue.svg</t>
   </si>
   <si>
     <t>Deanship of Graduate Studies</t>
@@ -635,6 +632,15 @@
   </si>
   <si>
     <t>College of Applied Studies</t>
+  </si>
+  <si>
+    <t>https://uobhomesiteprod.s3.me-south-1.amazonaws.com/site-prod/uploads/%D9%81%D8%B6%D9%84_%D8%A7%D9%84%D8%A8%D9%88%D8%B9%D9%8A%D9%86%D9%8A%D9%86-200x300.png</t>
+  </si>
+  <si>
+    <t>https://uobhomesiteprod.s3.me-south-1.amazonaws.com/site-prod/uploads/qTbPc9gA-Dr-Amel-Reg-Dean-2022-e1747810135468.jpg</t>
+  </si>
+  <si>
+    <t>https://www.undp.org/sites/g/files/zskgke326/files/2025-04/undp-logo-blue.4f32e17f.svg</t>
   </si>
 </sst>
 </file>
@@ -719,7 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -730,7 +736,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -739,9 +744,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1048,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView topLeftCell="L8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1128,7 +1131,7 @@
         <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>18</v>
@@ -1178,7 +1181,7 @@
         <v>30</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M2" s="2">
         <v>43466</v>
@@ -1202,7 +1205,7 @@
         <v>33</v>
       </c>
       <c r="U2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="V2">
         <v>26.2285</v>
@@ -1245,8 +1248,8 @@
       <c r="K3" t="s">
         <v>40</v>
       </c>
-      <c r="L3" t="s">
-        <v>41</v>
+      <c r="L3" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="M3" s="2">
         <v>44561</v>
@@ -1255,7 +1258,7 @@
         <v>45656</v>
       </c>
       <c r="O3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P3">
         <v>10</v>
@@ -1267,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T3" t="s">
         <v>33</v>
@@ -1293,13 +1296,13 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -1317,7 +1320,7 @@
         <v>30</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M4" s="2">
         <v>43466</v>
@@ -1338,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="S4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T4" t="s">
         <v>33</v>
@@ -1364,13 +1367,13 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
         <v>46</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
       </c>
       <c r="G5" t="s">
         <v>34</v>
@@ -1387,8 +1390,8 @@
       <c r="K5" t="s">
         <v>40</v>
       </c>
-      <c r="L5" t="s">
-        <v>41</v>
+      <c r="L5" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="M5" s="2">
         <v>44561</v>
@@ -1397,7 +1400,7 @@
         <v>46021</v>
       </c>
       <c r="O5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="P5">
         <v>10</v>
@@ -1409,7 +1412,7 @@
         <v>2</v>
       </c>
       <c r="S5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T5" t="s">
         <v>33</v>
@@ -1435,13 +1438,13 @@
         <v>35</v>
       </c>
       <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
         <v>49</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
@@ -1459,7 +1462,7 @@
         <v>30</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M6" s="2">
         <v>43466</v>
@@ -1503,16 +1506,16 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
         <v>51</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>52</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
       </c>
       <c r="G7" t="s">
         <v>34</v>
@@ -1529,8 +1532,8 @@
       <c r="K7" t="s">
         <v>40</v>
       </c>
-      <c r="L7" t="s">
-        <v>41</v>
+      <c r="L7" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="M7" s="2">
         <v>44561</v>
@@ -1539,7 +1542,7 @@
         <v>46386</v>
       </c>
       <c r="O7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P7">
         <v>10</v>
@@ -1551,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="S7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T7" t="s">
         <v>33</v>
@@ -1571,37 +1574,37 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
         <v>54</v>
       </c>
-      <c r="C8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>55</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
         <v>56</v>
       </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>57</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>58</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>59</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>60</v>
-      </c>
-      <c r="L8" t="s">
-        <v>61</v>
       </c>
       <c r="M8" s="2">
         <v>43831</v>
@@ -1610,7 +1613,7 @@
         <v>45291</v>
       </c>
       <c r="O8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P8">
         <v>8</v>
@@ -1622,7 +1625,7 @@
         <v>2</v>
       </c>
       <c r="S8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T8" t="s">
         <v>33</v>
@@ -1642,37 +1645,37 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
         <v>65</v>
       </c>
-      <c r="F9" t="s">
-        <v>66</v>
-      </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" t="s">
         <v>57</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>58</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>59</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>60</v>
-      </c>
-      <c r="L9" t="s">
-        <v>61</v>
       </c>
       <c r="M9" s="2">
         <v>43831</v>
@@ -1681,7 +1684,7 @@
         <v>45656</v>
       </c>
       <c r="O9" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="P9">
         <v>8</v>
@@ -1693,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="S9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T9" t="s">
         <v>33</v>
@@ -1713,10 +1716,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D10" t="s">
         <v>36</v>
@@ -1725,25 +1728,25 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" t="s">
         <v>57</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>58</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>59</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>60</v>
-      </c>
-      <c r="L10" t="s">
-        <v>61</v>
       </c>
       <c r="M10" s="2">
         <v>43831</v>
@@ -1752,7 +1755,7 @@
         <v>44926</v>
       </c>
       <c r="O10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P10">
         <v>8</v>
@@ -1764,7 +1767,7 @@
         <v>1</v>
       </c>
       <c r="S10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T10" t="s">
         <v>33</v>
@@ -1784,37 +1787,37 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
         <v>37</v>
       </c>
       <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" t="s">
         <v>69</v>
       </c>
-      <c r="G11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>70</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>71</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>72</v>
-      </c>
-      <c r="L11" t="s">
-        <v>73</v>
       </c>
       <c r="M11" s="2">
         <v>43831</v>
@@ -1823,7 +1826,7 @@
         <v>45656</v>
       </c>
       <c r="O11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P11">
         <v>3</v>
@@ -1835,7 +1838,7 @@
         <v>3</v>
       </c>
       <c r="S11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T11" t="s">
         <v>33</v>
@@ -1855,7 +1858,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
@@ -1864,28 +1867,28 @@
         <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" t="s">
         <v>70</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>71</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>72</v>
-      </c>
-      <c r="L12" t="s">
-        <v>73</v>
       </c>
       <c r="M12" s="2">
         <v>43831</v>
@@ -1894,7 +1897,7 @@
         <v>44926</v>
       </c>
       <c r="O12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P12">
         <v>3</v>
@@ -1906,7 +1909,7 @@
         <v>1</v>
       </c>
       <c r="S12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T12" t="s">
         <v>33</v>
@@ -1926,37 +1929,37 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" t="s">
         <v>70</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>71</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>72</v>
-      </c>
-      <c r="L13" t="s">
-        <v>73</v>
       </c>
       <c r="M13" s="2">
         <v>43831</v>
@@ -1965,7 +1968,7 @@
         <v>45291</v>
       </c>
       <c r="O13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P13">
         <v>3</v>
@@ -1977,7 +1980,7 @@
         <v>2</v>
       </c>
       <c r="S13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T13" t="s">
         <v>33</v>
@@ -1997,7 +2000,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
@@ -2006,28 +2009,28 @@
         <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" t="s">
         <v>77</v>
       </c>
-      <c r="G14" t="s">
-        <v>76</v>
-      </c>
-      <c r="H14" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>78</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>79</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>80</v>
-      </c>
-      <c r="L14" t="s">
-        <v>81</v>
       </c>
       <c r="M14" s="2">
         <v>44196</v>
@@ -2036,7 +2039,7 @@
         <v>45291</v>
       </c>
       <c r="O14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P14">
         <v>4</v>
@@ -2048,7 +2051,7 @@
         <v>1</v>
       </c>
       <c r="S14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T14" t="s">
         <v>33</v>
@@ -2068,37 +2071,37 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" t="s">
         <v>78</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>79</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>80</v>
-      </c>
-      <c r="L15" t="s">
-        <v>81</v>
       </c>
       <c r="M15" s="2">
         <v>44196</v>
@@ -2107,7 +2110,7 @@
         <v>45656</v>
       </c>
       <c r="O15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P15">
         <v>4</v>
@@ -2119,7 +2122,7 @@
         <v>2</v>
       </c>
       <c r="S15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T15" t="s">
         <v>33</v>
@@ -2139,37 +2142,37 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
         <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" t="s">
         <v>78</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>79</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>80</v>
-      </c>
-      <c r="L16" t="s">
-        <v>81</v>
       </c>
       <c r="M16" s="2">
         <v>44196</v>
@@ -2178,7 +2181,7 @@
         <v>46021</v>
       </c>
       <c r="O16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P16">
         <v>4</v>
@@ -2190,7 +2193,7 @@
         <v>3</v>
       </c>
       <c r="S16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T16" t="s">
         <v>33</v>
@@ -2210,37 +2213,37 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" t="s">
         <v>87</v>
       </c>
-      <c r="G17" t="s">
-        <v>86</v>
-      </c>
-      <c r="H17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>88</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>89</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>90</v>
-      </c>
-      <c r="L17" t="s">
-        <v>91</v>
       </c>
       <c r="M17" s="2">
         <v>43466</v>
@@ -2281,37 +2284,37 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" t="s">
         <v>92</v>
       </c>
-      <c r="F18" t="s">
-        <v>93</v>
-      </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I18" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" t="s">
         <v>88</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>89</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>90</v>
-      </c>
-      <c r="L18" t="s">
-        <v>91</v>
       </c>
       <c r="M18" s="2">
         <v>43466</v>
@@ -2352,7 +2355,7 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -2361,28 +2364,28 @@
         <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I19" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" t="s">
         <v>88</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>89</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>90</v>
-      </c>
-      <c r="L19" t="s">
-        <v>91</v>
       </c>
       <c r="M19" s="2">
         <v>43466</v>
@@ -2423,37 +2426,37 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" t="s">
         <v>96</v>
       </c>
-      <c r="G20" t="s">
-        <v>95</v>
-      </c>
-      <c r="H20" t="s">
-        <v>57</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>97</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>98</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>99</v>
-      </c>
-      <c r="L20" t="s">
-        <v>100</v>
       </c>
       <c r="M20" s="2">
         <v>44196</v>
@@ -2462,7 +2465,7 @@
         <v>46021</v>
       </c>
       <c r="O20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P20">
         <v>9</v>
@@ -2474,7 +2477,7 @@
         <v>3</v>
       </c>
       <c r="S20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T20" t="s">
         <v>33</v>
@@ -2494,7 +2497,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -2503,28 +2506,28 @@
         <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I21" t="s">
+        <v>96</v>
+      </c>
+      <c r="J21" t="s">
         <v>97</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>98</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>99</v>
-      </c>
-      <c r="L21" t="s">
-        <v>100</v>
       </c>
       <c r="M21" s="2">
         <v>44196</v>
@@ -2533,7 +2536,7 @@
         <v>45291</v>
       </c>
       <c r="O21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P21">
         <v>9</v>
@@ -2545,7 +2548,7 @@
         <v>1</v>
       </c>
       <c r="S21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T21" t="s">
         <v>33</v>
@@ -2565,37 +2568,37 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I22" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" t="s">
         <v>97</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>98</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>99</v>
-      </c>
-      <c r="L22" t="s">
-        <v>100</v>
       </c>
       <c r="M22" s="2">
         <v>44196</v>
@@ -2604,7 +2607,7 @@
         <v>45656</v>
       </c>
       <c r="O22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P22">
         <v>9</v>
@@ -2616,7 +2619,7 @@
         <v>2</v>
       </c>
       <c r="S22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T22" t="s">
         <v>33</v>
@@ -2636,37 +2639,37 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H23" t="s">
         <v>39</v>
       </c>
       <c r="I23" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23" t="s">
         <v>105</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>106</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>107</v>
-      </c>
-      <c r="L23" t="s">
-        <v>108</v>
       </c>
       <c r="M23" s="2">
         <v>44561</v>
@@ -2675,7 +2678,7 @@
         <v>46021</v>
       </c>
       <c r="O23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P23">
         <v>5</v>
@@ -2687,7 +2690,7 @@
         <v>2</v>
       </c>
       <c r="S23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T23" t="s">
         <v>33</v>
@@ -2707,37 +2710,37 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H24" t="s">
         <v>39</v>
       </c>
       <c r="I24" t="s">
+        <v>104</v>
+      </c>
+      <c r="J24" t="s">
         <v>105</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>106</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>107</v>
-      </c>
-      <c r="L24" t="s">
-        <v>108</v>
       </c>
       <c r="M24" s="2">
         <v>44561</v>
@@ -2746,7 +2749,7 @@
         <v>46386</v>
       </c>
       <c r="O24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P24">
         <v>5</v>
@@ -2758,7 +2761,7 @@
         <v>3</v>
       </c>
       <c r="S24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T24" t="s">
         <v>33</v>
@@ -2778,7 +2781,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -2787,28 +2790,28 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H25" t="s">
         <v>39</v>
       </c>
       <c r="I25" t="s">
+        <v>104</v>
+      </c>
+      <c r="J25" t="s">
         <v>105</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>106</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>107</v>
-      </c>
-      <c r="L25" t="s">
-        <v>108</v>
       </c>
       <c r="M25" s="2">
         <v>44561</v>
@@ -2817,7 +2820,7 @@
         <v>45656</v>
       </c>
       <c r="O25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P25">
         <v>5</v>
@@ -2829,7 +2832,7 @@
         <v>1</v>
       </c>
       <c r="S25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T25" t="s">
         <v>33</v>
@@ -2849,7 +2852,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
@@ -2858,28 +2861,28 @@
         <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" t="s">
+        <v>110</v>
+      </c>
+      <c r="H26" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" t="s">
         <v>112</v>
       </c>
-      <c r="G26" t="s">
-        <v>111</v>
-      </c>
-      <c r="H26" t="s">
-        <v>57</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>113</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>114</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>115</v>
-      </c>
-      <c r="L26" t="s">
-        <v>116</v>
       </c>
       <c r="M26" s="2">
         <v>43101</v>
@@ -2888,7 +2891,7 @@
         <v>44196</v>
       </c>
       <c r="O26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P26">
         <v>1</v>
@@ -2900,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="S26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T26" t="s">
         <v>33</v>
@@ -2920,37 +2923,37 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" t="s">
         <v>120</v>
       </c>
-      <c r="G27" t="s">
-        <v>119</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
+        <v>112</v>
+      </c>
+      <c r="J27" t="s">
         <v>121</v>
       </c>
-      <c r="I27" t="s">
-        <v>113</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>122</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>123</v>
-      </c>
-      <c r="L27" t="s">
-        <v>124</v>
       </c>
       <c r="M27" s="2">
         <v>43101</v>
@@ -2959,7 +2962,7 @@
         <v>44926</v>
       </c>
       <c r="O27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P27">
         <v>6</v>
@@ -2971,7 +2974,7 @@
         <v>3</v>
       </c>
       <c r="S27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T27" t="s">
         <v>33</v>
@@ -2991,37 +2994,37 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" t="s">
         <v>113</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>114</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>115</v>
-      </c>
-      <c r="L28" t="s">
-        <v>116</v>
       </c>
       <c r="M28" s="2">
         <v>43101</v>
@@ -3030,7 +3033,7 @@
         <v>44561</v>
       </c>
       <c r="O28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P28">
         <v>1</v>
@@ -3042,7 +3045,7 @@
         <v>2</v>
       </c>
       <c r="S28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T28" t="s">
         <v>33</v>
@@ -3062,7 +3065,7 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -3071,28 +3074,28 @@
         <v>36</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H29" t="s">
+        <v>120</v>
+      </c>
+      <c r="I29" t="s">
+        <v>112</v>
+      </c>
+      <c r="J29" t="s">
         <v>121</v>
       </c>
-      <c r="I29" t="s">
-        <v>113</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>122</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>123</v>
-      </c>
-      <c r="L29" t="s">
-        <v>124</v>
       </c>
       <c r="M29" s="2">
         <v>43101</v>
@@ -3101,7 +3104,7 @@
         <v>44196</v>
       </c>
       <c r="O29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P29">
         <v>6</v>
@@ -3113,7 +3116,7 @@
         <v>1</v>
       </c>
       <c r="S29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T29" t="s">
         <v>33</v>
@@ -3133,37 +3136,37 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
       <c r="D30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I30" t="s">
+        <v>112</v>
+      </c>
+      <c r="J30" t="s">
         <v>113</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>114</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>115</v>
-      </c>
-      <c r="L30" t="s">
-        <v>116</v>
       </c>
       <c r="M30" s="2">
         <v>43101</v>
@@ -3172,7 +3175,7 @@
         <v>44926</v>
       </c>
       <c r="O30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P30">
         <v>1</v>
@@ -3184,7 +3187,7 @@
         <v>3</v>
       </c>
       <c r="S30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T30" t="s">
         <v>33</v>
@@ -3204,37 +3207,37 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H31" t="s">
+        <v>120</v>
+      </c>
+      <c r="I31" t="s">
+        <v>112</v>
+      </c>
+      <c r="J31" t="s">
         <v>121</v>
       </c>
-      <c r="I31" t="s">
-        <v>113</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>122</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>123</v>
-      </c>
-      <c r="L31" t="s">
-        <v>124</v>
       </c>
       <c r="M31" s="2">
         <v>43101</v>
@@ -3243,7 +3246,7 @@
         <v>44561</v>
       </c>
       <c r="O31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P31">
         <v>6</v>
@@ -3255,7 +3258,7 @@
         <v>2</v>
       </c>
       <c r="S31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T31" t="s">
         <v>33</v>
@@ -3283,6 +3286,9 @@
     <hyperlink ref="L2" r:id="rId1" xr:uid="{F43ABA38-B1C2-42A5-8048-F0044B8A6906}"/>
     <hyperlink ref="L4" r:id="rId2" xr:uid="{D634AA35-232C-4686-8C28-A65DC64A39BC}"/>
     <hyperlink ref="L6" r:id="rId3" xr:uid="{6DC144AB-0F6A-465C-91E0-75F5AFD825CD}"/>
+    <hyperlink ref="L3" r:id="rId4" xr:uid="{7A71E4E0-F39E-4152-A9DE-8E955A6DBC78}"/>
+    <hyperlink ref="L5" r:id="rId5" xr:uid="{76800D4D-1357-40F5-9844-2ABE31CFBCF0}"/>
+    <hyperlink ref="L7" r:id="rId6" xr:uid="{A193A59A-0A4C-43BD-A30D-B986A95E8353}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3292,8 +3298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E120387-2C98-41B5-AA31-9226B0926BA8}">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3308,22 +3314,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -3331,19 +3337,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" t="s">
         <v>148</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>151</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -3351,71 +3357,74 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" t="s">
         <v>152</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="11" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" t="s">
         <v>159</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" t="s">
         <v>164</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -3423,19 +3432,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>172</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -3443,328 +3452,331 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="C8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11">
-        <v>8</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="C10" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="14" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="E13" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
-        <v>13</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="7"/>
+      <c r="B16" s="6"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B17" s="7"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B23" s="7"/>
+      <c r="B23" s="6"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B26" s="7"/>
+      <c r="B26" s="6"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B28" s="8"/>
+      <c r="B28" s="7"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B31" s="7"/>
+      <c r="B31" s="6"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B32" s="7"/>
+      <c r="B32" s="6"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B33" s="7"/>
+      <c r="B33" s="6"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B34" s="7"/>
+      <c r="B34" s="6"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B35" s="7"/>
+      <c r="B35" s="6"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B36" s="7"/>
+      <c r="B36" s="6"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B37" s="7"/>
+      <c r="B37" s="6"/>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B38" s="7"/>
+      <c r="B38" s="6"/>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B39" s="7"/>
+      <c r="B39" s="6"/>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B40" s="7"/>
+      <c r="B40" s="6"/>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B41" s="7"/>
+      <c r="B41" s="6"/>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B42" s="7"/>
+      <c r="B42" s="6"/>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B43" s="7"/>
+      <c r="B43" s="6"/>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B44" s="7"/>
+      <c r="B44" s="6"/>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B45" s="7"/>
+      <c r="B45" s="6"/>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B46" s="7"/>
+      <c r="B46" s="6"/>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B47" s="7"/>
+      <c r="B47" s="6"/>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B48" s="7"/>
+      <c r="B48" s="6"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="7"/>
+      <c r="B49" s="6"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="7"/>
+      <c r="B50" s="6"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="7"/>
+      <c r="B51" s="6"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" s="7"/>
+      <c r="B52" s="6"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" s="7"/>
+      <c r="B53" s="6"/>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" s="7"/>
+      <c r="B54" s="6"/>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B55" s="7"/>
+      <c r="B55" s="6"/>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" s="7"/>
+      <c r="B56" s="6"/>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B57" s="7"/>
+      <c r="B57" s="6"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" s="7"/>
+      <c r="B58" s="6"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" s="7"/>
+      <c r="B59" s="6"/>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="7"/>
+      <c r="B60" s="6"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="7"/>
+      <c r="B61" s="6"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="7"/>
+      <c r="B62" s="6"/>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" s="7"/>
+      <c r="B63" s="6"/>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B64" s="7"/>
+      <c r="B64" s="6"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" s="7"/>
+      <c r="B65" s="6"/>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" s="7"/>
+      <c r="B66" s="6"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" s="7"/>
+      <c r="B67" s="6"/>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" s="7"/>
+      <c r="B68" s="6"/>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B69" s="7"/>
+      <c r="B69" s="6"/>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B70" s="7"/>
+      <c r="B70" s="6"/>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B71" s="7"/>
+      <c r="B71" s="6"/>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B72" s="7"/>
+      <c r="B72" s="6"/>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B73" s="7"/>
+      <c r="B73" s="6"/>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B74" s="7"/>
+      <c r="B74" s="6"/>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B75" s="7"/>
+      <c r="B75" s="6"/>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B76" s="7"/>
+      <c r="B76" s="6"/>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B77" s="7"/>
+      <c r="B77" s="6"/>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B78" s="7"/>
+      <c r="B78" s="6"/>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B79" s="7"/>
+      <c r="B79" s="6"/>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B80" s="7"/>
+      <c r="B80" s="6"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B81" s="7"/>
+      <c r="B81" s="6"/>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B82" s="7"/>
+      <c r="B82" s="6"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B83" s="7"/>
+      <c r="B83" s="6"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B84" s="8"/>
+      <c r="B84" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -3789,6 +3801,8 @@
     <hyperlink ref="F12" r:id="rId18" xr:uid="{BD6894D3-FECF-4A3D-B66F-CBDA6DCE49A6}"/>
     <hyperlink ref="D13" r:id="rId19" tooltip="mailto:halarayedh@uob.edu.bh" display="mailto:halarayedh@uob.edu.bh" xr:uid="{D82AD61E-8142-4B97-AEAB-A4A862D47A9D}"/>
     <hyperlink ref="F13" r:id="rId20" xr:uid="{0D549E66-D75D-48F2-A1BF-13C300664E3D}"/>
+    <hyperlink ref="F14" r:id="rId21" xr:uid="{E6F5FAEB-AAC1-403A-BECA-E1D2851866BC}"/>
+    <hyperlink ref="F4" r:id="rId22" xr:uid="{B0E74BFA-7161-48ED-A086-261178316141}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Font changed, chart and stat style, leaders page style
</commit_message>
<xml_diff>
--- a/data/UoB_Agreements.xlsx
+++ b/data/UoB_Agreements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97333\Desktop\Hawra\Cloud Computing\ITCC481\Partnership\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6340EA1D-8D08-4C39-B8C5-729A00821DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C10E1C-CF9B-4958-8503-FF7842FDDE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,9 +474,6 @@
     <t>https://uobhomesiteprod.s3.me-south-1.amazonaws.com/site-prod/uploads/en/Dr.Fathima-1.jpg</t>
   </si>
   <si>
-    <t>Dr. Fatema Mohamed AlMalki</t>
-  </si>
-  <si>
     <t>Students Affairs</t>
   </si>
   <si>
@@ -486,9 +483,6 @@
     <t>+973 1743 8226</t>
   </si>
   <si>
-    <t>Dr. Salah Mohammed Ahmed</t>
-  </si>
-  <si>
     <t>College of Law</t>
   </si>
   <si>
@@ -501,15 +495,9 @@
     <t>+973 17438822</t>
   </si>
   <si>
-    <t>Dr. Amal Zayed Alzayed</t>
-  </si>
-  <si>
     <t>Admission and Registration</t>
   </si>
   <si>
-    <t>Dr. Athraa S.Abbas Al-Mosawi</t>
-  </si>
-  <si>
     <t>Graduate Studies &amp; Scientific Research</t>
   </si>
   <si>
@@ -522,10 +510,6 @@
     <t>+973 17438558</t>
   </si>
   <si>
-    <t xml:space="preserve">Dr. Leena Mohammad Abdulla Khonji
-</t>
-  </si>
-  <si>
     <t>College of Health and Sports Sciences</t>
   </si>
   <si>
@@ -541,9 +525,6 @@
     <t>+973 17435895</t>
   </si>
   <si>
-    <t>Dr. Haifa Ebrahim Al-Khalifa</t>
-  </si>
-  <si>
     <t>halkhalifa@uob.edu.bh</t>
   </si>
   <si>
@@ -553,9 +534,6 @@
     <t>https://uobhomesiteprod.s3.me-south-1.amazonaws.com/site-prod/uploads/engg/Sh-Dr-Haifa-Al-Khalifa-photo-1.jpg</t>
   </si>
   <si>
-    <t>Dr. Ali Salman Bin Thani</t>
-  </si>
-  <si>
     <t>abinthani@uob.edu.bh</t>
   </si>
   <si>
@@ -574,15 +552,9 @@
     <t>https://uobhomesiteprod.s3.me-south-1.amazonaws.com/site-prod/uploads/teachers/BTC-Dean-Dr.-Lucy-Baily-1.jpg</t>
   </si>
   <si>
-    <t>Dr. Abdulla Khalid Al-Jalahma</t>
-  </si>
-  <si>
     <t>https://uobhomesiteprod.s3.me-south-1.amazonaws.com/site-prod/uploads/cob/NbNfPtMk-6.jpg</t>
   </si>
   <si>
-    <t>Dr. Dheya Abdulla Al Kaabi</t>
-  </si>
-  <si>
     <t>dalkaabi@uob.edu.bh</t>
   </si>
   <si>
@@ -592,9 +564,6 @@
     <t>https://uobhomesiteprod.s3.me-south-1.amazonaws.com/site-prod/uploads/arts/2.jpg</t>
   </si>
   <si>
-    <t>Dr. Mazen Mohammed Ali</t>
-  </si>
-  <si>
     <t>mali@uob.edu.bh</t>
   </si>
   <si>
@@ -604,9 +573,6 @@
     <t>https://uobhomesiteprod.s3.me-south-1.amazonaws.com/sites/2/site-prod/uploads/DrMazenMohammedAli1.jpg</t>
   </si>
   <si>
-    <t>Dr. Hussain Muhsen Al Araydh</t>
-  </si>
-  <si>
     <t>halarayedh@uob.edu.bh</t>
   </si>
   <si>
@@ -616,9 +582,6 @@
     <t>https://uobhomesiteprod.s3.me-south-1.amazonaws.com/site-prod/uploads/cas/DrHussainAlArayedh.jpg</t>
   </si>
   <si>
-    <t>Mr. Fadhul Ghanem Al-buainain</t>
-  </si>
-  <si>
     <t>General Secretary of the University Council</t>
   </si>
   <si>
@@ -662,6 +625,42 @@
   </si>
   <si>
     <t>https://uobhomesiteprod.s3.me-south-1.amazonaws.com/site-prod/uploads/esraa.jpeg</t>
+  </si>
+  <si>
+    <t>Dr. Fatema AlMalki</t>
+  </si>
+  <si>
+    <t>Dr. Salah Ahmed</t>
+  </si>
+  <si>
+    <t>Dr. Amal Alzayed</t>
+  </si>
+  <si>
+    <t>Dr. Athraa Al-Mosawi</t>
+  </si>
+  <si>
+    <t>Dr. Leena Khonji</t>
+  </si>
+  <si>
+    <t>Dr. Haifa Al-Khalifa</t>
+  </si>
+  <si>
+    <t>Dr. Ali Bin Thani</t>
+  </si>
+  <si>
+    <t>Dr. Abdulla Al-Jalahma</t>
+  </si>
+  <si>
+    <t>Dr. Dheya Al Kaabi</t>
+  </si>
+  <si>
+    <t>Dr. Mazen Ali</t>
+  </si>
+  <si>
+    <t>Dr. Hussain Al Araydh</t>
+  </si>
+  <si>
+    <t>Mr. Fadhul Al-buainain</t>
   </si>
 </sst>
 </file>
@@ -746,7 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -767,10 +766,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1206,7 +1208,7 @@
         <v>30</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="M2" s="2">
         <v>43466</v>
@@ -1274,7 +1276,7 @@
         <v>40</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="M3" s="2">
         <v>44561</v>
@@ -1345,7 +1347,7 @@
         <v>30</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="M4" s="2">
         <v>43466</v>
@@ -1416,7 +1418,7 @@
         <v>40</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="M5" s="2">
         <v>44561</v>
@@ -1487,7 +1489,7 @@
         <v>30</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="M6" s="2">
         <v>43466</v>
@@ -1558,7 +1560,7 @@
         <v>40</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="M7" s="2">
         <v>44561</v>
@@ -1709,7 +1711,7 @@
         <v>45656</v>
       </c>
       <c r="O9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P9">
         <v>8</v>
@@ -3324,8 +3326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E120387-2C98-41B5-AA31-9226B0926BA8}">
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3358,7 +3360,7 @@
         <v>144</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3366,22 +3368,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C2" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="G2" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -3389,16 +3391,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" t="s">
         <v>146</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>145</v>
@@ -3409,19 +3411,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="C4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -3429,14 +3431,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>155</v>
+        <v>199</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="11" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -3444,39 +3446,39 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>161</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>162</v>
+      <c r="B7" s="14" t="s">
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -3484,19 +3486,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -3504,17 +3506,17 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C9" t="s">
         <v>81</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -3522,19 +3524,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -3542,14 +3544,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="11" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -3557,19 +3559,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="C12" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -3577,19 +3579,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="C13" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -3597,19 +3599,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="C14" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -3617,16 +3619,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added filter functionality to charts Removed unnecessary code for optimization Added animation to the Home page Fixed clear button to properly reset search input Added agreement type configuration object for marker colors and labels Updated displayed date format Changed map style
</commit_message>
<xml_diff>
--- a/data/UoB_Agreements.xlsx
+++ b/data/UoB_Agreements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97333\Desktop\Hawra\Cloud Computing\ITCC481\Partnership\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87776EC-8C64-4BCC-8E84-F70F01EC47AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09E582A5-00BC-4E30-BCAE-316ECD1635F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Leaders info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3327,7 +3328,7 @@
   <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3857,7 +3858,7 @@
     <hyperlink ref="F14" r:id="rId20" xr:uid="{0D549E66-D75D-48F2-A1BF-13C300664E3D}"/>
     <hyperlink ref="F15" r:id="rId21" xr:uid="{E6F5FAEB-AAC1-403A-BECA-E1D2851866BC}"/>
     <hyperlink ref="F5" r:id="rId22" xr:uid="{B0E74BFA-7161-48ED-A086-261178316141}"/>
-    <hyperlink ref="D2" r:id="rId23" tooltip="mailto:ewali@uob.edu.bh" display="mailto:ewali@uob.edu.bh" xr:uid="{E9FBF905-731A-4DED-A2A0-6BDABFF6B645}"/>
+    <hyperlink ref="D2" r:id="rId23" xr:uid="{E9FBF905-731A-4DED-A2A0-6BDABFF6B645}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>